<commit_message>
first comments on data
</commit_message>
<xml_diff>
--- a/data/ratios.xlsx
+++ b/data/ratios.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0025836\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5E0D256-F7E7-4FE9-82C9-C6230B703B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD1510C0-265D-45A3-9918-4B6F41847ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{412DA7F3-4624-4D19-B841-D3DA1309228D}"/>
   </bookViews>
   <sheets>
     <sheet name="ratios de prépa" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,6 +35,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E26454FD-67F5-4CCE-BDF1-9B289762FC8E}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E26454FD-67F5-4CCE-BDF1-9B289762FC8E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    moyennes temps d'éclatement 2023 / mois / type de marchandises, à comparer avec les moyennes qu'on peut calculer avec CEN.xlsx</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
@@ -51,7 +69,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,8 +121,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Tidiane Polo" id="{E15C74D2-3595-42C6-8DE9-5A2FB342050A}" userId="351fb774aae82982" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -398,20 +422,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2023-12-18T14:26:12.76" personId="{E15C74D2-3595-42C6-8DE9-5A2FB342050A}" id="{E26454FD-67F5-4CCE-BDF1-9B289762FC8E}">
+    <text>moyennes temps d'éclatement 2023 / mois / type de marchandises, à comparer avec les moyennes qu'on peut calculer avec CEN.xlsx</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3368BE42-EABF-47F8-8378-051A6B6AB175}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3368BE42-EABF-47F8-8378-051A6B6AB175}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="4" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -422,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>44927</v>
       </c>
@@ -436,7 +466,7 @@
         <v>199.3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>44958</v>
       </c>
@@ -450,7 +480,7 @@
         <v>194.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>44986</v>
       </c>
@@ -464,7 +494,7 @@
         <v>183.8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>45017</v>
       </c>
@@ -478,7 +508,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>45047</v>
       </c>
@@ -492,7 +522,7 @@
         <v>190.6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>45078</v>
       </c>
@@ -506,7 +536,7 @@
         <v>164.1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>45108</v>
       </c>
@@ -520,7 +550,7 @@
         <v>220.4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>45139</v>
       </c>
@@ -534,7 +564,7 @@
         <v>186.3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>45170</v>
       </c>
@@ -548,7 +578,7 @@
         <v>185.1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>45200</v>
       </c>
@@ -562,12 +592,12 @@
         <v>190.6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>45231</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>45261</v>
       </c>
@@ -575,10 +605,26 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FBF491DB27D134095CB75E07985203A" ma:contentTypeVersion="3" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0f435b4d933ff0fc367bd70e4b0d2749">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="22e37ad6-ebda-4163-bcf1-18ef8c6f6d6f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="606cc5398d19793d2bdb845cfbe038f5" ns2:_="">
     <xsd:import namespace="22e37ad6-ebda-4163-bcf1-18ef8c6f6d6f"/>
@@ -716,23 +762,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D566E7B-1EC8-4CF9-8DE1-D2FAE303F9F2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB505E8-CA7D-4C4A-AD01-A6A5D2F184A2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -740,5 +771,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB505E8-CA7D-4C4A-AD01-A6A5D2F184A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D566E7B-1EC8-4CF9-8DE1-D2FAE303F9F2}"/>
 </file>
</xml_diff>